<commit_message>
Enhance batch add certificate feature
</commit_message>
<xml_diff>
--- a/public/template-batch-upload.xlsx
+++ b/public/template-batch-upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bima.abadi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bimaj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80212013-D859-48C3-924C-971D68E8FB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7F61D5-4F12-46D4-888D-F75B9600575F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3DEB1B6B-CDB2-4D3C-89D3-AF75085E2D65}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3DEB1B6B-CDB2-4D3C-89D3-AF75085E2D65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Profesi Keuangan Expo 2022</t>
   </si>
@@ -44,28 +43,34 @@
     <t>Bima Jatmiko Abadi</t>
   </si>
   <si>
-    <t>KEGIATAN</t>
-  </si>
-  <si>
-    <t>NOMOR SERTIFIKAT</t>
-  </si>
-  <si>
-    <t>JUDUL WEBINAR</t>
-  </si>
-  <si>
-    <t>DURASI WEBINAR</t>
-  </si>
-  <si>
-    <t>NAMA PESERTA</t>
-  </si>
-  <si>
     <t>(Baris ini hanya contoh, mohon dihapus)</t>
   </si>
   <si>
-    <t>PKE-PPPK/2022/10879/1/10063</t>
-  </si>
-  <si>
     <t>Semua Bisa Cuan dengan Lelang Digital</t>
+  </si>
+  <si>
+    <t>ROLE</t>
+  </si>
+  <si>
+    <t>Peserta</t>
+  </si>
+  <si>
+    <t>TANGGAL SERTIFIKAT</t>
+  </si>
+  <si>
+    <t>2023-07-31</t>
+  </si>
+  <si>
+    <t>EXPO</t>
+  </si>
+  <si>
+    <t>JUDUL KEGIATAN</t>
+  </si>
+  <si>
+    <t>DURASI KEGIATAN</t>
+  </si>
+  <si>
+    <t>NAMA</t>
   </si>
 </sst>
 </file>
@@ -123,12 +128,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,56 +455,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405EE0E3-A390-4601-AA7C-DCEB8E7F18AA}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.21875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -502,18 +520,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -688,6 +706,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82474D12-4C79-4B63-9402-330A8BC8ED8E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39A381CD-AA9D-4D1D-B7C5-86362528528F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -700,14 +726,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82474D12-4C79-4B63-9402-330A8BC8ED8E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>